<commit_message>
lab 4 report shit
</commit_message>
<xml_diff>
--- a/lab4/experiment1DataAndCharts.xlsx
+++ b/lab4/experiment1DataAndCharts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="Chart3" sheetId="4" r:id="rId3"/>
     <sheet name="Chart4" sheetId="5" r:id="rId4"/>
     <sheet name="Chart5" sheetId="6" r:id="rId5"/>
-    <sheet name="experiment1Data.csv" sheetId="1" r:id="rId6"/>
+    <sheet name="Chart6" sheetId="7" r:id="rId6"/>
+    <sheet name="experiment1Data.csv" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Vbase</t>
   </si>
@@ -163,10 +164,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7910,6 +7912,51 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Collector Current Difference From Mean</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -10380,8 +10427,27 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Base Voltage (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00000E+00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2136260296"/>
@@ -10396,8 +10462,27 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent Difference (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00000E+00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2136263432"/>
@@ -11648,6 +11733,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Beta Values of Transistors</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -14228,8 +14332,12 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00000E+00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2092109368"/>
@@ -14244,11 +14352,2722 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Beta Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00000E+00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2092008664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Beta Values</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>experiment1Data.csv!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T1 Beta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$B$2:$B$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5E-9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.47E-8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.01E-8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.85E-8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.83E-8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.37E-8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.216E-7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.81E-7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.71E-7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4E-7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.88E-7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.64E-7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.259E-6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.812E-6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.78E-6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.02E-6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.79E-6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.31E-6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.183E-5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.676E-5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.17E-5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$G$2:$G$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.909090909090909</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.533333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.647058823529412</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.842105263157895</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.526315789473684</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.619047619047619</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.611111111111111</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.434782608695652</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.619047619047619</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.809523809523809</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.809523809523809</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.826086956521739</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.407407407407407</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.347826086956522</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.173913043478261</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.379310344827586</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10.13793103448276</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.96969696969697</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>31.96428571428572</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41.90322580645161</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>67.07142857142857</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>103.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>221.7948717948718</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>360.8571428571429</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>438.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>550.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>591.1764705882352</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>709.6385542168675</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>790.8256880733945</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>855.78231292517</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>911.9402985074626</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>964.9122807017544</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>982.885085574572</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1006.861063464837</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1021.505376344086</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1031.25</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1030.386740331492</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1033.210332103321</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1032.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1035.714285714286</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1033.564814814815</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1031.771247021446</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1028.69757174393</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1010.791366906475</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1009.950248756219</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1008.635578583765</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1004.813477737665</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>997.4640743871512</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>989.856801909308</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>850.8333333333333</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>628.3076923076923</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>628.3076923076923</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>628.3076923076923</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>628.3076923076923</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>626.3803680981596</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>626.3803680981596</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>626.3803680981596</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>626.3803680981596</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>624.4648318042813</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>624.4648318042813</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>624.4648318042813</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>622.5609756097561</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>622.5609756097561</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>620.6686930091186</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>620.6686930091186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>experiment1Data.csv!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T2 Beta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$B$2:$B$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5E-9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.47E-8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.01E-8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.85E-8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.83E-8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.37E-8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.216E-7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.81E-7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.71E-7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4E-7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.88E-7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.64E-7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.259E-6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.812E-6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.78E-6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.02E-6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.79E-6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.31E-6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.183E-5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.676E-5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.17E-5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$N$2:$N$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>2.267676767676767</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.47244094488189</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.586956521739131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.753623188405797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.176470588235294</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.162790697674419</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.277777777777777</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.421052631578948</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.90909090909091</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-14.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-4.142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-2.625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.583333333333333</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.916666666666666</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>18.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16.3529411764706</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>27.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43.14285714285714</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>55.1875</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>106.25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>141.4615384615385</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>178.6363636363637</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>247.3913043478261</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>391.4285714285714</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>397.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>556.1290322580645</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>772.7272727272727</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>687.037037037037</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>770.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>899.9999999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>931.967213114754</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>941.1428571428571</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>995.9349593495936</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1025.936599423631</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1040.241448692153</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1046.02510460251</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1054.474708171206</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1052.736982643525</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1043.859649122807</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1051.051051051051</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1053.27868852459</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1048.951048951049</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1047.984644913628</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1045.062955599735</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1026.200873362445</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1027.272727272727</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1023.157894736842</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1019.117647058824</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1012.383900928792</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1005.860805860806</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>997.3794549266245</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>759.1078066914498</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>experiment1Data.csv!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T3 Beta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$B$2:$B$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5E-9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.47E-8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.01E-8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.85E-8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.83E-8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.37E-8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.216E-7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.81E-7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.71E-7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4E-7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.88E-7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.64E-7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.259E-6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.812E-6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.78E-6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.02E-6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.79E-6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.31E-6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.183E-5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.676E-5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.17E-5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$U$2:$U$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>2.329896907216495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.59349593495935</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.793103448275862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.911764705882352</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.545454545454545</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.294117647058823</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.071428571428572</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-8.599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4.428571428571429</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.75</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.571428571428572</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.076923076923077</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.21428571428572</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21.57894736842105</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>50.83333333333334</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>68.38461538461537</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>75.82352941176471</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>109.1764705882353</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>228.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>188.5714285714286</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>249.1304347826087</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>359.5652173913044</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>428.2142857142858</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>559.6774193548387</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>640.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>731.3725490196078</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>785.5072463768116</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>865.934065934066</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>907.1428571428572</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>945.7142857142856</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>991.9354838709678</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1022.922636103152</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1025.742574257426</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1031.550068587106</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1046.242774566474</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1048.40848806366</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1039.130434782609</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1041.543026706232</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1040.485829959514</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1038.781163434903</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1037.986704653371</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1033.398821218075</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1017.316017316017</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1015.015015015015</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1014.613778705637</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1008.746355685131</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1004.098360655738</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>996.3662790697674</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>988.0395215808632</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>753.5055350553504</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>628.3076923076923</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>628.3076923076923</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>628.3076923076923</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>626.3803680981596</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>626.3803680981596</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>626.3803680981596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>experiment1Data.csv!$AB$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T4 Beta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$B$2:$B$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2E-9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6E-9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.1E-9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.7E-9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9E-9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.5E-9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.2E-9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5E-9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.8E-9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.3E-9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.47E-8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.01E-8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.85E-8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.09E-8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.83E-8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.37E-8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.216E-7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.81E-7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.71E-7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4E-7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.88E-7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.64E-7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.259E-6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.812E-6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.78E-6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.02E-6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.79E-6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.31E-6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.183E-5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.676E-5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.17E-5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.22E-5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.23E-5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.25E-5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.28E-5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.29E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>experiment1Data.csv!$AB$2:$AB$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.717277486910995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.897196261682243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.043478260869565</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.120689655172413</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.391304347826087</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.594594594594595</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.777777777777777</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.916666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.095238095238095</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.933333333333333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.083333333333333</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.428571428571429</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.58333333333333</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35.16666666666666</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36.53846153846154</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>53.38461538461538</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>84.41666666666667</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>145.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>178.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>181.7647058823529</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>223.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>307.1428571428571</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>464.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>537.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>605.625</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>755.2631578947369</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>706.7796610169491</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>929.2307692307691</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>911.4583333333332</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>925.5474452554745</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>994.0217391304348</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1026.415094339623</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1018.087855297158</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1040.072859744991</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1045.51201011378</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1048.28797190518</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1055.089820359281</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1048.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1046.321525885559</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1050.467289719626</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1045.977011494253</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1043.057996485061</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1040.14598540146</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1020.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1022.284122562674</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1019.417475728155</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1014.945652173913</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1007.670182166827</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1000.683994528044</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>991.1504424778762</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>719.0140845070422</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>646.2025316455696</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>644.1640378548897</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>642.1383647798742</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>640.1253918495297</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>636.1370716510903</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>634.1614906832299</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>632.1981424148607</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>630.2469135802469</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>638.233181529475</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2052804632"/>
+        <c:axId val="-2052459144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2052804632"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Base Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2052459144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2052459144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Beta</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2052804632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14310,6 +17129,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="143" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -14429,6 +17259,33 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8570280" cy="5826014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -14777,10 +17634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD101"/>
+  <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U1" activeCellId="4" sqref="A1:A1048576 G1:G1048576 N1:N1048576 AB1:AB1048576 U1:U1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14792,20 +17649,21 @@
     <col min="6" max="7" width="19.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="1"/>
     <col min="9" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" style="1"/>
     <col min="16" max="20" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5" style="1" customWidth="1"/>
     <col min="22" max="22" width="10.83203125" style="1"/>
     <col min="23" max="26" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.5" style="1" customWidth="1"/>
     <col min="29" max="29" width="10.83203125" style="1"/>
     <col min="30" max="30" width="18.5" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="31" max="31" width="10.83203125" style="1"/>
+    <col min="33" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:32">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14884,8 +17742,11 @@
       <c r="AD1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="AF1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:32">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -14981,8 +17842,11 @@
         <f>(E2+L2+S2+Z2)/4</f>
         <v>-1.6700000000000001E-8</v>
       </c>
+      <c r="AF2" s="3">
+        <v>1.12E-7</v>
+      </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:32">
       <c r="A3" s="1">
         <v>0.01</v>
       </c>
@@ -15078,8 +17942,11 @@
         <f t="shared" ref="AD3:AD66" si="16">(E3+L3+S3+Z3)/4</f>
         <v>-1.2925000000000003E-8</v>
       </c>
+      <c r="AF3" s="3">
+        <v>1.3E-7</v>
+      </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:32">
       <c r="A4" s="1">
         <v>0.02</v>
       </c>
@@ -15175,8 +18042,11 @@
         <f t="shared" si="16"/>
         <v>-1.0275000000000001E-8</v>
       </c>
+      <c r="AF4" s="3">
+        <v>1.8E-7</v>
+      </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:32">
       <c r="A5" s="1">
         <v>0.03</v>
       </c>
@@ -15272,8 +18142,11 @@
         <f t="shared" si="16"/>
         <v>-8.7500000000000006E-9</v>
       </c>
+      <c r="AF5" s="3">
+        <v>1.5300000000000001E-7</v>
+      </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:32">
       <c r="A6" s="1">
         <v>0.04</v>
       </c>
@@ -15369,8 +18242,11 @@
         <f t="shared" si="16"/>
         <v>-7.4750000000000008E-9</v>
       </c>
+      <c r="AF6" s="3">
+        <v>1.2800000000000001E-7</v>
+      </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:32">
       <c r="A7" s="1">
         <v>0.05</v>
       </c>
@@ -15466,8 +18342,11 @@
         <f t="shared" si="16"/>
         <v>-6.7000000000000004E-9</v>
       </c>
+      <c r="AF7" s="3">
+        <v>1.1999999999999999E-7</v>
+      </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:32">
       <c r="A8" s="1">
         <v>0.06</v>
       </c>
@@ -15563,8 +18442,11 @@
         <f t="shared" si="16"/>
         <v>-5.9750000000000006E-9</v>
       </c>
+      <c r="AF8" s="3">
+        <v>1.7100000000000001E-7</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:32">
       <c r="A9" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -15660,8 +18542,11 @@
         <f t="shared" si="16"/>
         <v>-5.6999999999999998E-9</v>
       </c>
+      <c r="AF9" s="3">
+        <v>2.7E-8</v>
+      </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:32">
       <c r="A10" s="1">
         <v>0.08</v>
       </c>
@@ -15757,8 +18642,11 @@
         <f t="shared" si="16"/>
         <v>-5.0999999999999993E-9</v>
       </c>
+      <c r="AF10" s="3">
+        <v>7.8999999999999996E-9</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:32">
       <c r="A11" s="1">
         <v>0.09</v>
       </c>
@@ -15854,8 +18742,11 @@
         <f t="shared" si="16"/>
         <v>-4.7749999999999997E-9</v>
       </c>
+      <c r="AF11" s="3">
+        <v>1.28E-8</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:32">
       <c r="A12" s="1">
         <v>0.1</v>
       </c>
@@ -15951,8 +18842,11 @@
         <f t="shared" si="16"/>
         <v>-4.6500000000000003E-9</v>
       </c>
+      <c r="AF12" s="3">
+        <v>4.3700000000000001E-8</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:32">
       <c r="A13" s="1">
         <v>0.11</v>
       </c>
@@ -16048,8 +18942,11 @@
         <f t="shared" si="16"/>
         <v>-4.1999999999999996E-9</v>
       </c>
+      <c r="AF13" s="3">
+        <v>6.4700000000000004E-8</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:32">
       <c r="A14" s="1">
         <v>0.12</v>
       </c>
@@ -16145,8 +19042,11 @@
         <f t="shared" si="16"/>
         <v>-4.0000000000000002E-9</v>
       </c>
+      <c r="AF14" s="3">
+        <v>6.5099999999999994E-8</v>
+      </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:32">
       <c r="A15" s="1">
         <v>0.13</v>
       </c>
@@ -16242,8 +19142,11 @@
         <f t="shared" si="16"/>
         <v>-3.7749999999999999E-9</v>
       </c>
+      <c r="AF15" s="3">
+        <v>6.3500000000000006E-8</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:32">
       <c r="A16" s="1">
         <v>0.14000000000000001</v>
       </c>
@@ -16339,8 +19242,11 @@
         <f t="shared" si="16"/>
         <v>-3.65E-9</v>
       </c>
+      <c r="AF16" s="3">
+        <v>7.3000000000000005E-8</v>
+      </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:32">
       <c r="A17" s="1">
         <v>0.15</v>
       </c>
@@ -16436,8 +19342,11 @@
         <f t="shared" si="16"/>
         <v>-3.4749999999999997E-9</v>
       </c>
+      <c r="AF17" s="3">
+        <v>6.8900000000000002E-8</v>
+      </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:32">
       <c r="A18" s="1">
         <v>0.16</v>
       </c>
@@ -16482,7 +19391,7 @@
         <v>22.777777777777779</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="7"/>
+        <f>K18/I18</f>
         <v>-14.000000000000002</v>
       </c>
       <c r="P18" s="1">
@@ -16533,8 +19442,11 @@
         <f t="shared" si="16"/>
         <v>-3.4750000000000005E-9</v>
       </c>
+      <c r="AF18" s="3">
+        <v>7.1099999999999995E-8</v>
+      </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:32">
       <c r="A19" s="1">
         <v>0.17</v>
       </c>
@@ -16630,8 +19542,11 @@
         <f t="shared" si="16"/>
         <v>-3.1999999999999997E-9</v>
       </c>
+      <c r="AF19" s="3">
+        <v>8.1899999999999999E-8</v>
+      </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:32">
       <c r="A20" s="1">
         <v>0.18</v>
       </c>
@@ -16727,8 +19642,11 @@
         <f t="shared" si="16"/>
         <v>-2.8000000000000003E-9</v>
       </c>
+      <c r="AF20" s="3">
+        <v>8.2700000000000006E-8</v>
+      </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:32">
       <c r="A21" s="1">
         <v>0.19</v>
       </c>
@@ -16824,8 +19742,11 @@
         <f t="shared" si="16"/>
         <v>-2.6249999999999999E-9</v>
       </c>
+      <c r="AF21" s="3">
+        <v>6.5400000000000003E-8</v>
+      </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:32">
       <c r="A22" s="1">
         <v>0.2</v>
       </c>
@@ -16921,8 +19842,11 @@
         <f t="shared" si="16"/>
         <v>-2.0750000000000004E-9</v>
       </c>
+      <c r="AF22" s="3">
+        <v>4.3999999999999997E-8</v>
+      </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:32">
       <c r="A23" s="1">
         <v>0.21</v>
       </c>
@@ -17018,8 +19942,11 @@
         <f t="shared" si="16"/>
         <v>-1.5E-9</v>
       </c>
+      <c r="AF23" s="3">
+        <v>1.7E-8</v>
+      </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:32">
       <c r="A24" s="1">
         <v>0.22</v>
       </c>
@@ -17115,8 +20042,11 @@
         <f t="shared" si="16"/>
         <v>-1.0250000000000001E-9</v>
       </c>
+      <c r="AF24" s="3">
+        <v>-2.85E-8</v>
+      </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:32">
       <c r="A25" s="1">
         <v>0.23</v>
       </c>
@@ -17212,8 +20142,11 @@
         <f t="shared" si="16"/>
         <v>9.9999999999999952E-11</v>
       </c>
+      <c r="AF25" s="3">
+        <v>-6.6600000000000001E-8</v>
+      </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:32">
       <c r="A26" s="1">
         <v>0.24</v>
       </c>
@@ -17309,8 +20242,11 @@
         <f t="shared" si="16"/>
         <v>1.4249999999999999E-9</v>
       </c>
+      <c r="AF26" s="3">
+        <v>-8.9500000000000001E-8</v>
+      </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:32">
       <c r="A27" s="1">
         <v>0.25</v>
       </c>
@@ -17406,8 +20342,11 @@
         <f t="shared" si="16"/>
         <v>3.4000000000000003E-9</v>
       </c>
+      <c r="AF27" s="3">
+        <v>-9.8900000000000005E-8</v>
+      </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:32">
       <c r="A28" s="1">
         <v>0.26</v>
       </c>
@@ -17503,8 +20442,11 @@
         <f t="shared" si="16"/>
         <v>6.3500000000000006E-9</v>
       </c>
+      <c r="AF28" s="3">
+        <v>-6.3500000000000006E-8</v>
+      </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:32">
       <c r="A29" s="1">
         <v>0.27</v>
       </c>
@@ -17600,8 +20542,11 @@
         <f t="shared" si="16"/>
         <v>1.0249999999999999E-8</v>
       </c>
+      <c r="AF29" s="3">
+        <v>-6.9999999999999998E-9</v>
+      </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:32">
       <c r="A30" s="1">
         <v>0.28000000000000003</v>
       </c>
@@ -17697,8 +20642,11 @@
         <f t="shared" si="16"/>
         <v>1.6525000000000001E-8</v>
       </c>
+      <c r="AF30" s="3">
+        <v>1.2299999999999999E-8</v>
+      </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:32">
       <c r="A31" s="1">
         <v>0.28999999999999998</v>
       </c>
@@ -17794,8 +20742,11 @@
         <f t="shared" si="16"/>
         <v>2.5200000000000001E-8</v>
       </c>
+      <c r="AF31" s="3">
+        <v>2.7199999999999999E-8</v>
+      </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:32">
       <c r="A32" s="1">
         <v>0.3</v>
       </c>
@@ -17891,8 +20842,11 @@
         <f t="shared" si="16"/>
         <v>3.7774999999999999E-8</v>
       </c>
+      <c r="AF32" s="3">
+        <v>3.3099999999999999E-8</v>
+      </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:32">
       <c r="A33" s="1">
         <v>0.31</v>
       </c>
@@ -17988,8 +20942,11 @@
         <f t="shared" si="16"/>
         <v>5.6599999999999991E-8</v>
       </c>
+      <c r="AF33" s="3">
+        <v>3.6699999999999998E-8</v>
+      </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:32">
       <c r="A34" s="1">
         <v>0.32</v>
       </c>
@@ -18085,8 +21042,11 @@
         <f t="shared" si="16"/>
         <v>8.3550000000000004E-8</v>
       </c>
+      <c r="AF34" s="3">
+        <v>6.0399999999999998E-8</v>
+      </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:32">
       <c r="A35" s="1">
         <v>0.33</v>
       </c>
@@ -18182,8 +21142,11 @@
         <f t="shared" si="16"/>
         <v>1.2127500000000001E-7</v>
       </c>
+      <c r="AF35" s="3">
+        <v>1.003E-7</v>
+      </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:32">
       <c r="A36" s="1">
         <v>0.34</v>
       </c>
@@ -18279,8 +21242,11 @@
         <f t="shared" si="16"/>
         <v>1.76525E-7</v>
       </c>
+      <c r="AF36" s="3">
+        <v>2.0480000000000001E-7</v>
+      </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:32">
       <c r="A37" s="1">
         <v>0.35</v>
       </c>
@@ -18376,8 +21342,11 @@
         <f t="shared" si="16"/>
         <v>2.5887500000000002E-7</v>
       </c>
+      <c r="AF37" s="3">
+        <v>3.9999999999999998E-7</v>
+      </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:32">
       <c r="A38" s="1">
         <v>0.36</v>
       </c>
@@ -18473,8 +21442,11 @@
         <f t="shared" si="16"/>
         <v>3.7649999999999996E-7</v>
       </c>
+      <c r="AF38" s="3">
+        <v>8.7999999999999994E-9</v>
+      </c>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:32">
       <c r="A39" s="1">
         <v>0.37</v>
       </c>
@@ -18570,8 +21542,11 @@
         <f t="shared" si="16"/>
         <v>5.4584999999999993E-7</v>
       </c>
+      <c r="AF39" s="3">
+        <v>1.3999999999999999E-9</v>
+      </c>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:32">
       <c r="A40" s="1">
         <v>0.38</v>
       </c>
@@ -18667,8 +21642,11 @@
         <f t="shared" si="16"/>
         <v>7.89975E-7</v>
       </c>
+      <c r="AF40" s="3">
+        <v>7.2100000000000004E-8</v>
+      </c>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:32">
       <c r="A41" s="1">
         <v>0.39</v>
       </c>
@@ -18764,8 +21742,11 @@
         <f t="shared" si="16"/>
         <v>1.1469500000000001E-6</v>
       </c>
+      <c r="AF41" s="3">
+        <v>2.3199999999999998E-6</v>
+      </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:32">
       <c r="A42" s="1">
         <v>0.4</v>
       </c>
@@ -18861,8 +21842,11 @@
         <f t="shared" si="16"/>
         <v>1.6617749999999999E-6</v>
       </c>
+      <c r="AF42" s="3">
+        <v>-3.9400000000000001E-7</v>
+      </c>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:32">
       <c r="A43" s="1">
         <v>0.41</v>
       </c>
@@ -18958,8 +21942,11 @@
         <f t="shared" si="16"/>
         <v>2.451425E-6</v>
       </c>
+      <c r="AF43" s="3">
+        <v>-8.3000000000000002E-8</v>
+      </c>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:32">
       <c r="A44" s="1">
         <v>0.42</v>
       </c>
@@ -19055,8 +22042,11 @@
         <f t="shared" si="16"/>
         <v>3.5846499999999996E-6</v>
       </c>
+      <c r="AF44" s="3">
+        <v>-1.63E-8</v>
+      </c>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:32">
       <c r="A45" s="1">
         <v>0.43</v>
       </c>
@@ -19152,8 +22142,11 @@
         <f t="shared" si="16"/>
         <v>5.2106999999999999E-6</v>
       </c>
+      <c r="AF45" s="3">
+        <v>4.8300000000000002E-8</v>
+      </c>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:32">
       <c r="A46" s="1">
         <v>0.44</v>
       </c>
@@ -19249,8 +22242,11 @@
         <f t="shared" si="16"/>
         <v>7.5785749999999997E-6</v>
       </c>
+      <c r="AF46" s="3">
+        <v>2.0480000000000001E-7</v>
+      </c>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:32">
       <c r="A47" s="1">
         <v>0.45</v>
       </c>
@@ -19346,8 +22342,11 @@
         <f t="shared" si="16"/>
         <v>1.101265E-5</v>
       </c>
+      <c r="AF47" s="3">
+        <v>-1.208E-7</v>
+      </c>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:32">
       <c r="A48" s="1">
         <v>0.46</v>
       </c>
@@ -19443,8 +22442,11 @@
         <f t="shared" si="16"/>
         <v>1.5955474999999998E-5</v>
       </c>
+      <c r="AF48" s="3">
+        <v>7.6599999999999998E-8</v>
+      </c>
     </row>
-    <row r="49" spans="1:30">
+    <row r="49" spans="1:32">
       <c r="A49" s="1">
         <v>0.47</v>
       </c>
@@ -19540,8 +22542,11 @@
         <f t="shared" si="16"/>
         <v>2.36335E-5</v>
       </c>
+      <c r="AF49" s="3">
+        <v>5.3500000000000003E-8</v>
+      </c>
     </row>
-    <row r="50" spans="1:30">
+    <row r="50" spans="1:32">
       <c r="A50" s="1">
         <v>0.48</v>
       </c>
@@ -19637,8 +22642,11 @@
         <f t="shared" si="16"/>
         <v>3.4515799999999999E-5</v>
       </c>
+      <c r="AF50" s="3">
+        <v>7.7400000000000005E-8</v>
+      </c>
     </row>
-    <row r="51" spans="1:30">
+    <row r="51" spans="1:32">
       <c r="A51" s="1">
         <v>0.49</v>
       </c>
@@ -19734,8 +22742,11 @@
         <f t="shared" si="16"/>
         <v>5.0151000000000001E-5</v>
       </c>
+      <c r="AF51" s="3">
+        <v>5.1800000000000001E-8</v>
+      </c>
     </row>
-    <row r="52" spans="1:30">
+    <row r="52" spans="1:32">
       <c r="A52" s="1">
         <v>0.5</v>
       </c>
@@ -19831,8 +22842,11 @@
         <f t="shared" si="16"/>
         <v>7.2829499999999984E-5</v>
       </c>
+      <c r="AF52" s="3">
+        <v>6.8400000000000004E-8</v>
+      </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:32">
       <c r="A53" s="1">
         <v>0.51</v>
       </c>
@@ -19928,8 +22942,11 @@
         <f t="shared" si="16"/>
         <v>1.0537395000000001E-4</v>
       </c>
+      <c r="AF53" s="3">
+        <v>8.6700000000000002E-8</v>
+      </c>
     </row>
-    <row r="54" spans="1:30">
+    <row r="54" spans="1:32">
       <c r="A54" s="1">
         <v>0.52</v>
       </c>
@@ -20025,8 +23042,11 @@
         <f t="shared" si="16"/>
         <v>1.5420270000000001E-4</v>
       </c>
+      <c r="AF54" s="3">
+        <v>9.0299999999999995E-8</v>
+      </c>
     </row>
-    <row r="55" spans="1:30">
+    <row r="55" spans="1:32">
       <c r="A55" s="1">
         <v>0.53</v>
       </c>
@@ -20122,8 +23142,11 @@
         <f t="shared" si="16"/>
         <v>2.3115275000000002E-4</v>
       </c>
+      <c r="AF55" s="3">
+        <v>1.062E-7</v>
+      </c>
     </row>
-    <row r="56" spans="1:30">
+    <row r="56" spans="1:32">
       <c r="A56" s="1">
         <v>0.54</v>
       </c>
@@ -20219,8 +23242,11 @@
         <f t="shared" si="16"/>
         <v>3.4092299999999997E-4</v>
       </c>
+      <c r="AF56" s="3">
+        <v>8.7499999999999996E-8</v>
+      </c>
     </row>
-    <row r="57" spans="1:30">
+    <row r="57" spans="1:32">
       <c r="A57" s="1">
         <v>0.55000000000000004</v>
       </c>
@@ -20316,8 +23342,11 @@
         <f t="shared" si="16"/>
         <v>5.0027075000000007E-4</v>
       </c>
+      <c r="AF57" s="3">
+        <v>8.3200000000000004E-8</v>
+      </c>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:32">
       <c r="A58" s="1">
         <v>0.56000000000000005</v>
       </c>
@@ -20413,8 +23442,11 @@
         <f t="shared" si="16"/>
         <v>7.3129800000000002E-4</v>
       </c>
+      <c r="AF58" s="3">
+        <v>8.9200000000000005E-8</v>
+      </c>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:32">
       <c r="A59" s="1">
         <v>0.56999999999999995</v>
       </c>
@@ -20510,8 +23542,11 @@
         <f t="shared" si="16"/>
         <v>1.0652257500000002E-3</v>
       </c>
+      <c r="AF59" s="3">
+        <v>9.1899999999999996E-8</v>
+      </c>
     </row>
-    <row r="60" spans="1:30">
+    <row r="60" spans="1:32">
       <c r="A60" s="1">
         <v>0.57999999999999996</v>
       </c>
@@ -20607,8 +23642,11 @@
         <f t="shared" si="16"/>
         <v>1.5395152499999998E-3</v>
       </c>
+      <c r="AF60" s="3">
+        <v>9.5599999999999996E-8</v>
+      </c>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:32">
       <c r="A61" s="1">
         <v>0.59</v>
       </c>
@@ -20704,8 +23742,11 @@
         <f t="shared" si="16"/>
         <v>2.2762720000000002E-3</v>
       </c>
+      <c r="AF61" s="3">
+        <v>1.023E-7</v>
+      </c>
     </row>
-    <row r="62" spans="1:30">
+    <row r="62" spans="1:32">
       <c r="A62" s="1">
         <v>0.6</v>
       </c>
@@ -20801,8 +23842,11 @@
         <f t="shared" si="16"/>
         <v>3.3092500000000001E-3</v>
       </c>
+      <c r="AF62" s="3">
+        <v>9.4199999999999996E-8</v>
+      </c>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:32">
       <c r="A63" s="1">
         <v>0.61</v>
       </c>
@@ -20898,8 +23942,11 @@
         <f t="shared" si="16"/>
         <v>4.7528225E-3</v>
       </c>
+      <c r="AF63" s="3">
+        <v>1.247E-7</v>
+      </c>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:32">
       <c r="A64" s="1">
         <v>0.62</v>
       </c>
@@ -20995,8 +24042,11 @@
         <f t="shared" si="16"/>
         <v>6.7832975000000004E-3</v>
       </c>
+      <c r="AF64" s="3">
+        <v>2.0600000000000002E-6</v>
+      </c>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:32">
       <c r="A65" s="1">
         <v>0.63</v>
       </c>
@@ -21092,8 +24142,11 @@
         <f t="shared" si="16"/>
         <v>9.6079524999999992E-3</v>
       </c>
+      <c r="AF65" s="3">
+        <v>1.946E-5</v>
+      </c>
     </row>
-    <row r="66" spans="1:30">
+    <row r="66" spans="1:32">
       <c r="A66" s="1">
         <v>0.64</v>
       </c>
@@ -21189,8 +24242,11 @@
         <f t="shared" si="16"/>
         <v>1.3454035E-2</v>
       </c>
+      <c r="AF66" s="3">
+        <v>1.9749999999999999E-5</v>
+      </c>
     </row>
-    <row r="67" spans="1:30">
+    <row r="67" spans="1:32">
       <c r="A67" s="1">
         <v>0.65</v>
       </c>
@@ -21286,8 +24342,11 @@
         <f t="shared" ref="AD67:AD101" si="33">(E67+L67+S67+Z67)/4</f>
         <v>1.86761475E-2</v>
       </c>
+      <c r="AF67">
+        <v>2.0599999999999999E-4</v>
+      </c>
     </row>
-    <row r="68" spans="1:30">
+    <row r="68" spans="1:32">
       <c r="A68" s="1">
         <v>0.66</v>
       </c>
@@ -21383,8 +24442,11 @@
         <f t="shared" si="33"/>
         <v>2.0393399999999999E-2</v>
       </c>
+      <c r="AF68">
+        <v>5.9699999999999998E-4</v>
+      </c>
     </row>
-    <row r="69" spans="1:30">
+    <row r="69" spans="1:32">
       <c r="A69" s="1">
         <v>0.67</v>
       </c>
@@ -21480,8 +24542,11 @@
         <f t="shared" si="33"/>
         <v>2.0388299999999998E-2</v>
       </c>
+      <c r="AF69">
+        <v>7.67E-4</v>
+      </c>
     </row>
-    <row r="70" spans="1:30">
+    <row r="70" spans="1:32">
       <c r="A70" s="1">
         <v>0.68</v>
       </c>
@@ -21577,8 +24642,11 @@
         <f t="shared" si="33"/>
         <v>2.0388150000000001E-2</v>
       </c>
+      <c r="AF70">
+        <v>9.8299999999999993E-4</v>
+      </c>
     </row>
-    <row r="71" spans="1:30">
+    <row r="71" spans="1:32">
       <c r="A71" s="1">
         <v>0.69</v>
       </c>
@@ -21674,8 +24742,11 @@
         <f t="shared" si="33"/>
         <v>2.0388175000000001E-2</v>
       </c>
+      <c r="AF71">
+        <v>1.2539999999999999E-3</v>
+      </c>
     </row>
-    <row r="72" spans="1:30">
+    <row r="72" spans="1:32">
       <c r="A72" s="1">
         <v>0.7</v>
       </c>
@@ -21771,8 +24842,11 @@
         <f t="shared" si="33"/>
         <v>2.0388175000000001E-2</v>
       </c>
+      <c r="AF72">
+        <v>1.596E-3</v>
+      </c>
     </row>
-    <row r="73" spans="1:30">
+    <row r="73" spans="1:32">
       <c r="A73" s="1">
         <v>0.71</v>
       </c>
@@ -21868,8 +24942,11 @@
         <f t="shared" si="33"/>
         <v>2.0388175000000001E-2</v>
       </c>
+      <c r="AF73">
+        <v>2.0349999999999999E-3</v>
+      </c>
     </row>
-    <row r="74" spans="1:30">
+    <row r="74" spans="1:32">
       <c r="A74" s="1">
         <v>0.72</v>
       </c>
@@ -21965,8 +25042,11 @@
         <f t="shared" si="33"/>
         <v>2.0388150000000001E-2</v>
       </c>
+      <c r="AF74">
+        <v>2.6700000000000001E-3</v>
+      </c>
     </row>
-    <row r="75" spans="1:30">
+    <row r="75" spans="1:32">
       <c r="A75" s="1">
         <v>0.73</v>
       </c>
@@ -22062,8 +25142,11 @@
         <f t="shared" si="33"/>
         <v>2.0388125E-2</v>
       </c>
+      <c r="AF75">
+        <v>3.3400000000000001E-3</v>
+      </c>
     </row>
-    <row r="76" spans="1:30">
+    <row r="76" spans="1:32">
       <c r="A76" s="1">
         <v>0.74</v>
       </c>
@@ -22159,8 +25242,11 @@
         <f t="shared" si="33"/>
         <v>2.0388125E-2</v>
       </c>
+      <c r="AF76">
+        <v>4.1700000000000001E-3</v>
+      </c>
     </row>
-    <row r="77" spans="1:30">
+    <row r="77" spans="1:32">
       <c r="A77" s="1">
         <v>0.75</v>
       </c>
@@ -22256,8 +25342,11 @@
         <f t="shared" si="33"/>
         <v>2.0388125E-2</v>
       </c>
+      <c r="AF77">
+        <v>5.1500000000000001E-3</v>
+      </c>
     </row>
-    <row r="78" spans="1:30">
+    <row r="78" spans="1:32">
       <c r="A78" s="1">
         <v>0.76</v>
       </c>
@@ -22353,8 +25442,11 @@
         <f t="shared" si="33"/>
         <v>2.0388100000000003E-2</v>
       </c>
+      <c r="AF78">
+        <v>6.3299999999999997E-3</v>
+      </c>
     </row>
-    <row r="79" spans="1:30">
+    <row r="79" spans="1:32">
       <c r="A79" s="1">
         <v>0.77</v>
       </c>
@@ -22450,8 +25542,11 @@
         <f t="shared" si="33"/>
         <v>2.0388075000000002E-2</v>
       </c>
+      <c r="AF79">
+        <v>7.7200000000000003E-3</v>
+      </c>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:32">
       <c r="A80" s="1">
         <v>0.78</v>
       </c>
@@ -22547,8 +25642,11 @@
         <f t="shared" si="33"/>
         <v>2.0388025000000004E-2</v>
       </c>
+      <c r="AF80">
+        <v>9.3299999999999998E-3</v>
+      </c>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:32">
       <c r="A81" s="1">
         <v>0.79</v>
       </c>
@@ -22644,8 +25742,11 @@
         <f t="shared" si="33"/>
         <v>2.0388025000000004E-2</v>
       </c>
+      <c r="AF81">
+        <v>1.115E-2</v>
+      </c>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:32">
       <c r="A82" s="1">
         <v>0.8</v>
       </c>
@@ -22741,8 +25842,11 @@
         <f t="shared" si="33"/>
         <v>2.0388000000000003E-2</v>
       </c>
+      <c r="AF82">
+        <v>1.319E-2</v>
+      </c>
     </row>
-    <row r="83" spans="1:30">
+    <row r="83" spans="1:32">
       <c r="A83" s="1">
         <v>0.81</v>
       </c>
@@ -22838,8 +25942,11 @@
         <f t="shared" si="33"/>
         <v>2.0387975000000003E-2</v>
       </c>
+      <c r="AF83">
+        <v>1.5429999999999999E-2</v>
+      </c>
     </row>
-    <row r="84" spans="1:30">
+    <row r="84" spans="1:32">
       <c r="A84" s="1">
         <v>0.82</v>
       </c>
@@ -22935,8 +26042,11 @@
         <f t="shared" si="33"/>
         <v>2.0387975000000003E-2</v>
       </c>
+      <c r="AF84">
+        <v>1.7860000000000001E-2</v>
+      </c>
     </row>
-    <row r="85" spans="1:30">
+    <row r="85" spans="1:32">
       <c r="A85" s="1">
         <v>0.83</v>
       </c>
@@ -23032,8 +26142,11 @@
         <f t="shared" si="33"/>
         <v>2.0387925000000001E-2</v>
       </c>
+      <c r="AF85">
+        <v>2.043E-2</v>
+      </c>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:32">
       <c r="A86" s="1">
         <v>0.84</v>
       </c>
@@ -23129,8 +26242,11 @@
         <f t="shared" si="33"/>
         <v>2.03879E-2</v>
       </c>
+      <c r="AF86">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="87" spans="1:30">
+    <row r="87" spans="1:32">
       <c r="A87" s="1">
         <v>0.85</v>
       </c>
@@ -23226,8 +26342,11 @@
         <f t="shared" si="33"/>
         <v>2.0387875E-2</v>
       </c>
+      <c r="AF87">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:32">
       <c r="A88" s="1">
         <v>0.86</v>
       </c>
@@ -23323,8 +26442,11 @@
         <f t="shared" si="33"/>
         <v>2.0387849999999999E-2</v>
       </c>
+      <c r="AF88">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="89" spans="1:30">
+    <row r="89" spans="1:32">
       <c r="A89" s="1">
         <v>0.87</v>
       </c>
@@ -23420,8 +26542,11 @@
         <f t="shared" si="33"/>
         <v>2.0387825000000002E-2</v>
       </c>
+      <c r="AF89">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:32">
       <c r="A90" s="1">
         <v>0.88</v>
       </c>
@@ -23517,8 +26642,11 @@
         <f t="shared" si="33"/>
         <v>2.0387800000000001E-2</v>
       </c>
+      <c r="AF90">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="91" spans="1:30">
+    <row r="91" spans="1:32">
       <c r="A91" s="1">
         <v>0.89</v>
       </c>
@@ -23614,8 +26742,11 @@
         <f t="shared" si="33"/>
         <v>2.0387725000000002E-2</v>
       </c>
+      <c r="AF91">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:32">
       <c r="A92" s="1">
         <v>0.9</v>
       </c>
@@ -23711,8 +26842,11 @@
         <f t="shared" si="33"/>
         <v>2.0387725000000002E-2</v>
       </c>
+      <c r="AF92">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="93" spans="1:30">
+    <row r="93" spans="1:32">
       <c r="A93" s="1">
         <v>0.91</v>
       </c>
@@ -23808,8 +26942,11 @@
         <f t="shared" si="33"/>
         <v>2.0387700000000002E-2</v>
       </c>
+      <c r="AF93">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="94" spans="1:30">
+    <row r="94" spans="1:32">
       <c r="A94" s="1">
         <v>0.92</v>
       </c>
@@ -23905,8 +27042,11 @@
         <f t="shared" si="33"/>
         <v>2.038765E-2</v>
       </c>
+      <c r="AF94">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:32">
       <c r="A95" s="1">
         <v>0.93</v>
       </c>
@@ -24002,8 +27142,11 @@
         <f t="shared" si="33"/>
         <v>2.0387624999999999E-2</v>
       </c>
+      <c r="AF95">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="96" spans="1:30">
+    <row r="96" spans="1:32">
       <c r="A96" s="1">
         <v>0.94</v>
       </c>
@@ -24099,8 +27242,11 @@
         <f t="shared" si="33"/>
         <v>2.0387599999999999E-2</v>
       </c>
+      <c r="AF96">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="97" spans="1:30">
+    <row r="97" spans="1:32">
       <c r="A97" s="1">
         <v>0.95</v>
       </c>
@@ -24196,8 +27342,11 @@
         <f t="shared" si="33"/>
         <v>2.0387574999999998E-2</v>
       </c>
+      <c r="AF97">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:32">
       <c r="A98" s="1">
         <v>0.96</v>
       </c>
@@ -24293,8 +27442,11 @@
         <f t="shared" si="33"/>
         <v>2.0387525000000004E-2</v>
       </c>
+      <c r="AF98">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="99" spans="1:30">
+    <row r="99" spans="1:32">
       <c r="A99" s="1">
         <v>0.97</v>
       </c>
@@ -24390,8 +27542,11 @@
         <f t="shared" si="33"/>
         <v>2.0387475000000002E-2</v>
       </c>
+      <c r="AF99">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="100" spans="1:30">
+    <row r="100" spans="1:32">
       <c r="A100" s="1">
         <v>0.98</v>
       </c>
@@ -24487,8 +27642,11 @@
         <f t="shared" si="33"/>
         <v>2.0387425000000001E-2</v>
       </c>
+      <c r="AF100">
+        <v>2.0619999999999999E-2</v>
+      </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:32">
       <c r="A101" s="1">
         <v>0.99</v>
       </c>
@@ -24583,6 +27741,18 @@
       <c r="AD101" s="1">
         <f t="shared" si="33"/>
         <v>2.0387425000000001E-2</v>
+      </c>
+      <c r="AF101">
+        <v>2.0619999999999999E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:32">
+      <c r="AB102" s="1">
+        <f>AVERAGE(AB75:AB101)</f>
+        <v>638.23318152947513</v>
+      </c>
+      <c r="AF102">
+        <v>2.0619999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>